<commit_message>
modified 70 crawl questions
</commit_message>
<xml_diff>
--- a/train003.xlsx
+++ b/train003.xlsx
@@ -607,14 +607,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="119.5" customWidth="1"/>
     <col min="3" max="24" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>